<commit_message>
Updated to create csv output
</commit_message>
<xml_diff>
--- a/protocol_info.xlsx
+++ b/protocol_info.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_info" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,35 +17,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
-  <si>
-    <t>0060</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+  <si>
+    <t>0046</t>
+  </si>
+  <si>
+    <t>0052</t>
+  </si>
+  <si>
+    <t>0048</t>
+  </si>
+  <si>
+    <t>0051</t>
+  </si>
+  <si>
+    <t>0037</t>
+  </si>
+  <si>
+    <t>0067</t>
+  </si>
+  <si>
+    <t>0054</t>
+  </si>
+  <si>
+    <t>0053</t>
+  </si>
+  <si>
+    <t>0068</t>
+  </si>
+  <si>
+    <t>0044</t>
+  </si>
+  <si>
+    <t>0050</t>
+  </si>
+  <si>
+    <t>A251</t>
+  </si>
+  <si>
+    <t>0059</t>
+  </si>
+  <si>
+    <t>0055</t>
+  </si>
+  <si>
+    <t>0062</t>
+  </si>
+  <si>
+    <t>0047</t>
+  </si>
+  <si>
+    <t>0079I</t>
+  </si>
+  <si>
+    <t>0049</t>
   </si>
   <si>
     <t>0064</t>
   </si>
   <si>
-    <t>0068</t>
+    <t>0071</t>
+  </si>
+  <si>
+    <t>0073</t>
   </si>
   <si>
     <t>0069</t>
   </si>
   <si>
-    <t>0071</t>
-  </si>
-  <si>
-    <t>0067</t>
-  </si>
-  <si>
-    <t>0079</t>
-  </si>
-  <si>
-    <t>0079I</t>
-  </si>
-  <si>
-    <t>0073</t>
-  </si>
-  <si>
     <t>0069I</t>
   </si>
   <si>
@@ -53,9 +92,6 @@
   </si>
   <si>
     <t>0075S</t>
-  </si>
-  <si>
-    <t>MVR01</t>
   </si>
   <si>
     <t>CTN-NODES</t>
@@ -410,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,7 +454,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:26">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,93 +494,201 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>2</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
+      <c r="T2" t="n">
+        <v>7</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" t="n">
+        <v>4</v>
+      </c>
+      <c r="X2" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
         <v>6</v>
       </c>
-      <c r="F2" t="n">
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>11</v>
+      </c>
+      <c r="T3" t="n">
+        <v>11</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" t="n">
         <v>4</v>
       </c>
-      <c r="G2" t="n">
-        <v>7</v>
-      </c>
-      <c r="H2" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="X3" t="n">
         <v>4</v>
       </c>
-      <c r="L2" t="n">
-        <v>3</v>
-      </c>
-      <c r="M2" t="n">
-        <v>3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="n">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>30</v>
-      </c>
-      <c r="D3" t="n">
-        <v>20</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n">
-        <v>8</v>
-      </c>
-      <c r="G3" t="n">
-        <v>14</v>
-      </c>
-      <c r="H3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I3" t="n">
-        <v>6</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="n">
-        <v>8</v>
-      </c>
-      <c r="L3" t="n">
-        <v>6</v>
-      </c>
-      <c r="M3" t="n">
-        <v>6</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2</v>
+      <c r="Y3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>